<commit_message>
Report Daily Sales Checking
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateDailySalesCheckingBase.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateDailySalesCheckingBase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\Documents\SourceProjects\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C514B42-8340-4A0B-A06E-21C5C64856C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6664EAC0-7944-4BC8-B640-46C3E9692495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="1095" windowWidth="24240" windowHeight="13140" xr2:uid="{440ECAD8-9E77-4B0E-86CD-E9E348C2B6A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{440ECAD8-9E77-4B0E-86CD-E9E348C2B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Template1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Daily Sales Checking Report - Base</t>
   </si>
@@ -71,10 +71,6 @@
 (On Date of Sale)</t>
   </si>
   <si>
-    <t>Actual Premium
-(On Date of Sale)</t>
-  </si>
-  <si>
     <t>Actual Children
 (On Date of Sale)</t>
   </si>
@@ -130,6 +126,14 @@
   </si>
   <si>
     <t>Original Date of Sale</t>
+  </si>
+  <si>
+    <t>Actual LA2 
+(On Date of Sale)</t>
+  </si>
+  <si>
+    <t>Actual Premium 
+(On Date of Sale)</t>
   </si>
 </sst>
 </file>
@@ -389,15 +393,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,20 +717,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380709B0-1E99-494F-806A-7DF58DDC74A0}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.85546875" customWidth="1"/>
-    <col min="2" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="4.85546875" customWidth="1"/>
+    <col min="2" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -745,10 +749,11 @@
       <c r="N1" s="26"/>
       <c r="O1" s="26"/>
       <c r="P1" s="26"/>
-      <c r="Q1" s="27"/>
-    </row>
-    <row r="2" spans="1:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="26"/>
+      <c r="R1" s="27"/>
+    </row>
+    <row r="2" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
@@ -767,10 +772,11 @@
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29"/>
-      <c r="Q3" s="27"/>
-    </row>
-    <row r="4" spans="1:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q3" s="29"/>
+      <c r="R3" s="27"/>
+    </row>
+    <row r="4" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>2</v>
       </c>
@@ -789,32 +795,34 @@
       <c r="N5" s="29"/>
       <c r="O5" s="29"/>
       <c r="P5" s="29"/>
-      <c r="Q5" s="27"/>
-    </row>
-    <row r="6" spans="1:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="Q5" s="29"/>
+      <c r="R5" s="27"/>
+    </row>
+    <row r="6" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="27"/>
-    </row>
-    <row r="8" spans="1:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:17" ht="106.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="33"/>
+    </row>
+    <row r="8" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" ht="106.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -833,84 +841,89 @@
       <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="R9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="7"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="8"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="15"/>
-    </row>
-    <row r="12" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="11"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="15"/>
+    </row>
+    <row r="12" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="17">
-        <f t="shared" ref="B12:I12" si="0">SUM(B10:B10)</f>
+        <f t="shared" ref="B12:J12" si="0">SUM(B10:B10)</f>
         <v>0</v>
       </c>
       <c r="C12" s="18">
@@ -928,115 +941,122 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
+        <f>SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0</v>
+      </c>
+      <c r="I12" s="18">
+        <f t="shared" ref="I12" si="1">SUM(I10:I10)</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="18">
-        <f t="shared" ref="H12" si="1">SUM(H10:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="18">
-        <v>0</v>
-      </c>
-      <c r="K12" s="17">
-        <v>0</v>
-      </c>
-      <c r="L12" s="18">
-        <f>SUM(L$10:L10)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="17">
+      <c r="K12" s="18">
+        <v>0</v>
+      </c>
+      <c r="L12" s="17">
+        <v>0</v>
+      </c>
+      <c r="M12" s="18">
         <f>SUM(M$10:M10)</f>
         <v>0</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="17">
         <f>SUM(N$10:N10)</f>
         <v>0</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12" s="18">
         <f>SUM(O$10:O10)</f>
         <v>0</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="17">
         <f>SUM(P$10:P10)</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="18">
+        <f>SUM(Q$10:Q10)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-    </row>
-    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+    </row>
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33" t="s">
+      <c r="E16" s="32"/>
+      <c r="F16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="22" t="s">
+      <c r="G16" s="22"/>
+      <c r="H16" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="24"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A3:Q3"/>
-    <mergeCell ref="A5:Q5"/>
-    <mergeCell ref="A7:Q7"/>
-    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="A5:R5"/>
+    <mergeCell ref="A7:R7"/>
+    <mergeCell ref="A15:J15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="H16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Daily Sales checking referrals column added
Daily Sales checking referrals column added to summary and batch code splits
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateDailySalesCheckingBase.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateDailySalesCheckingBase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\source\repos\Insure20230223\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B2740F-4885-46C2-B757-2D99388D9857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D98438-21B5-477E-9F89-03958DF09CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>TOTALS</t>
   </si>
@@ -128,6 +128,9 @@
   <si>
     <t>Actual LA2
 (On Date of Sale)</t>
+  </si>
+  <si>
+    <t>Total Referrals</t>
   </si>
 </sst>
 </file>
@@ -368,6 +371,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -375,9 +387,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,17 +394,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,10 +705,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:R7"/>
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,101 +716,105 @@
     <col min="1" max="1" width="42.85546875" customWidth="1"/>
     <col min="2" max="17" width="10" customWidth="1"/>
     <col min="18" max="18" width="4.85546875" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="27"/>
-    </row>
-    <row r="2" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+    </row>
+    <row r="2" spans="1:19" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="27"/>
-    </row>
-    <row r="4" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="29"/>
+    </row>
+    <row r="4" spans="1:19" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="27"/>
-    </row>
-    <row r="6" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+    </row>
+    <row r="6" spans="1:19" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="27"/>
-    </row>
-    <row r="8" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:18" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+    </row>
+    <row r="8" spans="1:19" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:19" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -864,8 +869,11 @@
       <c r="R9" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="14"/>
       <c r="C10" s="10"/>
@@ -884,8 +892,9 @@
       <c r="P10" s="14"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="22"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S10" s="32"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="15"/>
       <c r="C11" s="11"/>
@@ -904,8 +913,9 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="12"/>
       <c r="R11" s="21"/>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S11" s="32"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -970,8 +980,11 @@
       <c r="R12" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="S12" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -979,68 +992,68 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-    </row>
-    <row r="16" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="33"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="A5:S5"/>
+    <mergeCell ref="A7:S7"/>
+    <mergeCell ref="A1:S1"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="G16:J16"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A3:R3"/>
-    <mergeCell ref="A5:R5"/>
-    <mergeCell ref="A7:R7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>